<commit_message>
Started on grouping Students into Schedules
</commit_message>
<xml_diff>
--- a/scr/main/resources/data/StudentData.xlsx
+++ b/scr/main/resources/data/StudentData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mecha\Documents\GitHub\Invited-Meeting-Scheduler\scr\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A51A5F-C26A-4360-85D9-033C4062972D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CDF92D-702A-4D6B-BF08-209F51466FA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="4215" windowWidth="25080" windowHeight="11385" xr2:uid="{3F80A9F9-5585-4065-BFAC-5B8001948D72}"/>
+    <workbookView xWindow="2685" yWindow="4215" windowWidth="25080" windowHeight="11385" xr2:uid="{3F80A9F9-5585-4065-BFAC-5B8001948D72}"/>
   </bookViews>
   <sheets>
     <sheet name="RawData" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -121,7 +121,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -151,8 +150,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,10 +470,13 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -499,7 +502,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>111109</v>
       </c>
       <c r="B2" t="s">
@@ -521,9 +524,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>111110.0</v>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>111110</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>

</xml_diff>